<commit_message>
OFC Nations Cup 1996, 1998, 2000, 2002
OFC Nations Cup 1996, 1998, 2000, 2002
</commit_message>
<xml_diff>
--- a/Tournaments/Tournaments.xlsx
+++ b/Tournaments/Tournaments.xlsx
@@ -608,7 +608,7 @@
       <c r="F5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="1" t="str">
+      <c r="G5" s="2" t="str">
         <f>"- Juegos Olimpicos"</f>
         <v>- Juegos Olimpicos</v>
       </c>
@@ -747,6 +747,10 @@
       <c r="B10" s="1" t="str">
         <f>"- Eliminatorias Copa del Mundo Futsal"</f>
         <v>- Eliminatorias Copa del Mundo Futsal</v>
+      </c>
+      <c r="D10" s="1" t="str">
+        <f>"- Trans Tasman Cup"</f>
+        <v>- Trans Tasman Cup</v>
       </c>
       <c r="F10" s="1" t="str">
         <f>"- Eliminatorias Copa del Mundo Futsal"</f>

</xml_diff>

<commit_message>
Futsal World Cup Tournament
Futsal World Cup Tournament
</commit_message>
<xml_diff>
--- a/Tournaments/Tournaments.xlsx
+++ b/Tournaments/Tournaments.xlsx
@@ -463,7 +463,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -711,7 +713,7 @@
         <f>"- Eliminatorias Copa del Mundo Sub 20"</f>
         <v>- Eliminatorias Copa del Mundo Sub 20</v>
       </c>
-      <c r="G8" s="1" t="str">
+      <c r="G8" s="2" t="str">
         <f>"- Copa del Mundo Futsal"</f>
         <v>- Copa del Mundo Futsal</v>
       </c>

</xml_diff>

<commit_message>
Review Africa Cup of Nations
Review Africa Cup of Nations
</commit_message>
<xml_diff>
--- a/Tournaments/Tournaments.xlsx
+++ b/Tournaments/Tournaments.xlsx
@@ -463,9 +463,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -509,7 +507,7 @@
         <f>"- Eliminatorias Copa America"</f>
         <v>- Eliminatorias Copa America</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">

</xml_diff>

<commit_message>
African Nations Championship 2014, 2016
African Nations Championship 2014, 2016
</commit_message>
<xml_diff>
--- a/Tournaments/Tournaments.xlsx
+++ b/Tournaments/Tournaments.xlsx
@@ -549,7 +549,7 @@
       <c r="E3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="2" t="s">
         <v>19</v>
       </c>
       <c r="G3" s="1" t="str">
@@ -763,6 +763,10 @@
         <f>"- Juegos Paramericanos"</f>
         <v>- Juegos Paramericanos</v>
       </c>
+      <c r="H10" s="1" t="str">
+        <f>"- China Cup"</f>
+        <v>- China Cup</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D11" s="2" t="str">
@@ -793,11 +797,11 @@
         <v>9</v>
       </c>
       <c r="H12">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I12">
         <f>SUM(A12:H12)</f>
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>